<commit_message>
finished working with link to db
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13e8c7332eaaef2b/Документы/UiPath/GazpromTest/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D76C3245-5E7C-4A83-B3BF-81ECB4A8F307}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CC95D2D-CA87-4348-9493-50144404F9D4}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="1395" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="1680" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t>Here you need to write the information about the database</t>
+  </si>
+  <si>
+    <t>PathToPathon</t>
+  </si>
+  <si>
+    <t>C:\Users\jorov\anaconda3</t>
+  </si>
+  <si>
+    <t>PathToAttachments</t>
+  </si>
+  <si>
+    <t>C:\Users\jorov\OneDrive\Документы\UiPath\GazpromTest\Attachments</t>
   </si>
 </sst>
 </file>
@@ -413,7 +425,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="A3:C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -470,11 +482,22 @@
       </c>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="5" spans="1:26">
       <c r="C5" s="3"/>
     </row>

</xml_diff>